<commit_message>
Adding merge, fixing bug in combine latest and withNextFrom
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -827,7 +827,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1249,6 +1249,9 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
       <c r="B33" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Adding switchOnNext and tests
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1274,6 +1274,9 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
       <c r="B35" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Adding ElementAt and tests, removing unused constants
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="8505"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -827,7 +827,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1082,6 +1082,9 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
       <c r="B20" t="s">
         <v>70</v>
       </c>
@@ -1509,6 +1512,9 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
       <c r="B55" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Adding Timer and test
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -971,6 +971,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
       <c r="B11" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Adding CatchError and test
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -827,7 +827,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1308,6 +1308,9 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
       <c r="B37" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Adding every and contains and adding tests for and fixing bugs in publishTo, receiveFrom, observeOn
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1010,6 +1010,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
       <c r="B14" t="s">
         <v>69</v>
       </c>
@@ -1469,6 +1472,9 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
       <c r="B50" t="s">
         <v>74</v>
       </c>
@@ -1491,6 +1497,9 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
       <c r="B52" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Adding Concat, SkipWhile, TakeWhile
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1547,6 +1547,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>81</v>
+      </c>
       <c r="B56" t="s">
         <v>74</v>
       </c>
@@ -1572,6 +1575,9 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>81</v>
+      </c>
       <c r="B58" t="s">
         <v>74</v>
       </c>
@@ -1594,6 +1600,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>81</v>
+      </c>
       <c r="B60" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Adding Empty, Never, Error
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -826,7 +826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -874,6 +876,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
       <c r="B4" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Adding Count, Sum, ConcatString, Max, Min
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -827,7 +827,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1626,6 +1626,9 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>81</v>
+      </c>
       <c r="B61" t="s">
         <v>75</v>
       </c>
@@ -1673,6 +1676,9 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>81</v>
+      </c>
       <c r="B65" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Adding timestamp and updateTimestamp
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="150">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1459,6 +1459,9 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>81</v>
+      </c>
       <c r="B48" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Fixing FlatMap, SwitchOnNext. Adding SwitchMap, debounce and tests
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="14355" windowHeight="8385"/>
+    <workbookView xWindow="360" yWindow="210" windowWidth="14355" windowHeight="8325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="154">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -470,6 +470,18 @@
   </si>
   <si>
     <t>ensure that all observers see the same sequence of emitted items, even if they subscribe after the Observable has begun emitting items</t>
+  </si>
+  <si>
+    <t>emit an item from an Observable but do not emit another until a time window has passed</t>
+  </si>
+  <si>
+    <t>ThrottleFirst</t>
+  </si>
+  <si>
+    <t>ThrottleLast</t>
+  </si>
+  <si>
+    <t>when an item is  from an Observable but do not emit another until a time window has passed</t>
   </si>
 </sst>
 </file>
@@ -519,7 +531,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -824,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1066,6 +1092,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
       <c r="B18" t="s">
         <v>70</v>
       </c>
@@ -1165,38 +1194,32 @@
         <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>81</v>
-      </c>
       <c r="B26" t="s">
         <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>81</v>
-      </c>
       <c r="B27" t="s">
         <v>70</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1207,10 +1230,10 @@
         <v>70</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1221,21 +1244,24 @@
         <v>70</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1243,13 +1269,13 @@
         <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1257,10 +1283,10 @@
         <v>71</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1271,24 +1297,21 @@
         <v>71</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>81</v>
-      </c>
       <c r="B34" t="s">
         <v>71</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1299,10 +1322,10 @@
         <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1313,10 +1336,10 @@
         <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1324,13 +1347,13 @@
         <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1338,13 +1361,13 @@
         <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1352,13 +1375,13 @@
         <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1366,24 +1389,27 @@
         <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
       <c r="B41" t="s">
         <v>73</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1394,10 +1420,10 @@
         <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1405,10 +1431,10 @@
         <v>73</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1419,10 +1445,10 @@
         <v>73</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1430,10 +1456,10 @@
         <v>73</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1444,24 +1470,21 @@
         <v>73</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>81</v>
-      </c>
       <c r="B47" t="s">
         <v>73</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1472,21 +1495,24 @@
         <v>73</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>81</v>
+      </c>
       <c r="B49" t="s">
         <v>73</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1494,27 +1520,24 @@
         <v>81</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>81</v>
-      </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1525,10 +1548,10 @@
         <v>74</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1539,10 +1562,10 @@
         <v>74</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D53" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1553,10 +1576,10 @@
         <v>74</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1567,10 +1590,10 @@
         <v>74</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1581,10 +1604,10 @@
         <v>74</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D56" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1595,10 +1618,10 @@
         <v>74</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D57" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1609,10 +1632,10 @@
         <v>74</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D58" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1620,13 +1643,13 @@
         <v>81</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D59" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1634,13 +1657,13 @@
         <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1651,10 +1674,10 @@
         <v>75</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D61" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1665,10 +1688,10 @@
         <v>75</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D62" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1679,10 +1702,10 @@
         <v>75</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1693,10 +1716,10 @@
         <v>75</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1707,10 +1730,10 @@
         <v>75</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1718,13 +1741,13 @@
         <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D66" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1732,13 +1755,13 @@
         <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1749,10 +1772,10 @@
         <v>76</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D68" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -1763,16 +1786,44 @@
         <v>76</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D71" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
-  <conditionalFormatting sqref="A2:XFD69">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A2:XFD71">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>"Done"=$A2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding buffer, bufferTime, bufferCount, bufferTimeOrCount
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="154">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1014,6 +1014,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
       <c r="B12" t="s">
         <v>69</v>
       </c>
@@ -1081,6 +1084,9 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
       <c r="B17" t="s">
         <v>69</v>
       </c>
@@ -1190,6 +1196,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
       <c r="B25" t="s">
         <v>70</v>
       </c>
@@ -1201,6 +1210,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
       <c r="B26" t="s">
         <v>70</v>
       </c>
@@ -1212,6 +1224,9 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
       <c r="B27" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
adding pipeOn, pipeOnNewContext, subscribeOn, subscribeOnNewContext
</commit_message>
<xml_diff>
--- a/RxEpl - Done.xlsx
+++ b/RxEpl - Done.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="154">
   <si>
     <t xml:space="preserve">Create </t>
   </si>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1492,6 +1492,9 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>81</v>
+      </c>
       <c r="B47" t="s">
         <v>73</v>
       </c>

</xml_diff>